<commit_message>
update of appareal resource
</commit_message>
<xml_diff>
--- a/TestData/Register_Data.xlsx
+++ b/TestData/Register_Data.xlsx
@@ -44,13 +44,13 @@
     <t>${confirm_pass}</t>
   </si>
   <si>
-    <t>John</t>
+    <t>Bharath</t>
   </si>
   <si>
-    <t>JK</t>
+    <t>Kathir</t>
   </si>
   <si>
-    <t>john@gmail.com</t>
+    <t>bharath@gmail.com</t>
   </si>
   <si>
     <t>sivakami</t>
@@ -77,14 +77,15 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -529,26 +530,26 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -674,7 +675,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,7 +998,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1044,7 +1045,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="john@gmail.com" tooltip="mailto:john@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="bharath@gmail.com" tooltip="mailto:bharath@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>